<commit_message>
MUL, IMUL, DIV, IDIV
Реализованы соответствующие инструкции.
</commit_message>
<xml_diff>
--- a/Codes.xlsx
+++ b/Codes.xlsx
@@ -502,42 +502,6 @@
     <t>00</t>
   </si>
   <si>
-    <t>07 0s</t>
-  </si>
-  <si>
-    <t>07 1s</t>
-  </si>
-  <si>
-    <t>07 2s</t>
-  </si>
-  <si>
-    <t>07 4s</t>
-  </si>
-  <si>
-    <t>07 5s</t>
-  </si>
-  <si>
-    <t>07 6s</t>
-  </si>
-  <si>
-    <t>07 8s</t>
-  </si>
-  <si>
-    <t>07 9s</t>
-  </si>
-  <si>
-    <t>07 As</t>
-  </si>
-  <si>
-    <t>07 Cs</t>
-  </si>
-  <si>
-    <t>07 Ds</t>
-  </si>
-  <si>
-    <t>07 Es</t>
-  </si>
-  <si>
     <t>08 0s</t>
   </si>
   <si>
@@ -1178,6 +1142,42 @@
   </si>
   <si>
     <t>07 Ez</t>
+  </si>
+  <si>
+    <t>08 1i</t>
+  </si>
+  <si>
+    <t>08 2i</t>
+  </si>
+  <si>
+    <t>08 3i</t>
+  </si>
+  <si>
+    <t>08 9i</t>
+  </si>
+  <si>
+    <t>08 Ai</t>
+  </si>
+  <si>
+    <t>08 Bi</t>
+  </si>
+  <si>
+    <t>09 1i</t>
+  </si>
+  <si>
+    <t>09 2i</t>
+  </si>
+  <si>
+    <t>09 3i</t>
+  </si>
+  <si>
+    <t>09 9i</t>
+  </si>
+  <si>
+    <t>09 Ai</t>
+  </si>
+  <si>
+    <t>09 Bi</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1406,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1421,11 +1424,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1434,22 +1440,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54:D56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1795,58 +1795,58 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="D3" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="30"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D4" s="33"/>
+        <v>338</v>
+      </c>
+      <c r="D4" s="34"/>
       <c r="F4" s="2" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="30"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D5" s="33"/>
+        <v>339</v>
+      </c>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="30"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D6" s="33"/>
+        <v>340</v>
+      </c>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="31"/>
@@ -1854,43 +1854,43 @@
         <v>7</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="D7" s="34"/>
+        <v>341</v>
+      </c>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="D8" s="42" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="35"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D9" s="39"/>
+        <v>343</v>
+      </c>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="36"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="D10" s="40"/>
+        <v>344</v>
+      </c>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>22</v>
@@ -1909,45 +1909,45 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D13" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="35"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D14" s="39"/>
+        <v>327</v>
+      </c>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="35"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D15" s="39"/>
+        <v>328</v>
+      </c>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10" t="s">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>21</v>
@@ -1966,7 +1966,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>27</v>
@@ -1980,9 +1980,9 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D18" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="D18" s="33" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1992,297 +1992,297 @@
         <v>17</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="D19" s="34"/>
+        <v>330</v>
+      </c>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="30" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="D20" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="35"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D21" s="39"/>
+        <v>332</v>
+      </c>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D22" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="D22" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="35"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="D23" s="39"/>
+        <v>334</v>
+      </c>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="D24" s="39" t="s">
+        <v>335</v>
+      </c>
+      <c r="D24" s="42" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A25" s="36"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="D25" s="40"/>
+        <v>336</v>
+      </c>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="D26" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="D26" s="34" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="30"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D27" s="33"/>
+        <v>348</v>
+      </c>
+      <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="30"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D28" s="33"/>
+        <v>349</v>
+      </c>
+      <c r="D28" s="34"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="30"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D29" s="33"/>
+        <v>350</v>
+      </c>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="30"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="D30" s="33"/>
+        <v>351</v>
+      </c>
+      <c r="D30" s="34"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D31" s="39" t="s">
+        <v>352</v>
+      </c>
+      <c r="D31" s="42" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="35"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D32" s="39"/>
+        <v>353</v>
+      </c>
+      <c r="D32" s="42"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="35"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D33" s="39"/>
+        <v>354</v>
+      </c>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="35"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D34" s="39"/>
+        <v>355</v>
+      </c>
+      <c r="D34" s="42"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A35" s="36"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="D35" s="40"/>
+        <v>356</v>
+      </c>
+      <c r="D35" s="44"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="30" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>369</v>
-      </c>
-      <c r="D36" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="D36" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="35"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D37" s="39"/>
+        <v>358</v>
+      </c>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="35"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D38" s="39"/>
+        <v>359</v>
+      </c>
+      <c r="D38" s="42"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="35"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D39" s="39"/>
+        <v>360</v>
+      </c>
+      <c r="D39" s="42"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="35"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="D40" s="39"/>
+        <v>361</v>
+      </c>
+      <c r="D40" s="42"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D41" s="39" t="s">
+        <v>362</v>
+      </c>
+      <c r="D41" s="42" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="35"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D42" s="39"/>
+        <v>363</v>
+      </c>
+      <c r="D42" s="42"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="35"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D43" s="39"/>
+        <v>364</v>
+      </c>
+      <c r="D43" s="42"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="35"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D44" s="39"/>
+        <v>365</v>
+      </c>
+      <c r="D44" s="42"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A45" s="36"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="D45" s="40"/>
+        <v>366</v>
+      </c>
+      <c r="D45" s="44"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="45" t="s">
@@ -2292,85 +2292,85 @@
         <v>8</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="D46" s="46" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="35"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D47" s="39"/>
+        <v>368</v>
+      </c>
+      <c r="D47" s="42"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="35"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D48" s="39"/>
+        <v>369</v>
+      </c>
+      <c r="D48" s="42"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="35"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D49" s="39"/>
+        <v>370</v>
+      </c>
+      <c r="D49" s="42"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A50" s="36"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="D50" s="40"/>
+        <v>371</v>
+      </c>
+      <c r="D50" s="44"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="32" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D51" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="D51" s="34" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="30"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D52" s="33"/>
+        <v>373</v>
+      </c>
+      <c r="D52" s="34"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="41"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D53" s="42"/>
+        <v>374</v>
+      </c>
+      <c r="D53" s="36"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="29" t="s">
@@ -2380,21 +2380,21 @@
         <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D54" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="D54" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="30"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D55" s="33"/>
+        <v>376</v>
+      </c>
+      <c r="D55" s="34"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1">
       <c r="A56" s="31"/>
@@ -2402,43 +2402,43 @@
         <v>18</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="34"/>
+        <v>377</v>
+      </c>
+      <c r="D56" s="35"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="39" t="s">
         <v>49</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D57" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="D57" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="30"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D58" s="33"/>
+        <v>379</v>
+      </c>
+      <c r="D58" s="34"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="41"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" s="42"/>
+        <v>380</v>
+      </c>
+      <c r="D59" s="36"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="29" t="s">
@@ -2448,21 +2448,21 @@
         <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" s="32" t="s">
+        <v>381</v>
+      </c>
+      <c r="D60" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="30"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D61" s="33"/>
+        <v>382</v>
+      </c>
+      <c r="D61" s="34"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1">
       <c r="A62" s="31"/>
@@ -2470,21 +2470,21 @@
         <v>18</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D62" s="34"/>
+        <v>383</v>
+      </c>
+      <c r="D62" s="35"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="39" t="s">
         <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D63" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" s="40" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2494,161 +2494,161 @@
         <v>17</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="D64" s="34"/>
+        <v>159</v>
+      </c>
+      <c r="D64" s="35"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="32" t="s">
         <v>83</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D65" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D65" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="30"/>
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D66" s="33"/>
+        <v>161</v>
+      </c>
+      <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="30"/>
+      <c r="A67" s="32"/>
       <c r="B67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D67" s="33"/>
+        <v>162</v>
+      </c>
+      <c r="D67" s="34"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="30"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D68" s="33"/>
+        <v>163</v>
+      </c>
+      <c r="D68" s="34"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="30"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D69" s="33"/>
+        <v>164</v>
+      </c>
+      <c r="D69" s="34"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D70" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70" s="42" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="35"/>
+      <c r="A71" s="41"/>
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D71" s="39"/>
+        <v>166</v>
+      </c>
+      <c r="D71" s="42"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="35"/>
+      <c r="A72" s="41"/>
       <c r="B72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D72" s="39"/>
+        <v>167</v>
+      </c>
+      <c r="D72" s="42"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="35"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D73" s="39"/>
+        <v>168</v>
+      </c>
+      <c r="D73" s="42"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A74" s="36"/>
+      <c r="A74" s="43"/>
       <c r="B74" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D74" s="40"/>
+        <v>169</v>
+      </c>
+      <c r="D74" s="44"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="32" t="s">
         <v>57</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D75" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D75" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="30"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D76" s="33"/>
+        <v>178</v>
+      </c>
+      <c r="D76" s="34"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="30"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D77" s="33"/>
+        <v>175</v>
+      </c>
+      <c r="D77" s="34"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="30"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D78" s="33"/>
+        <v>170</v>
+      </c>
+      <c r="D78" s="34"/>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1">
       <c r="A79" s="31"/>
@@ -2656,53 +2656,53 @@
         <v>10</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="D79" s="34"/>
+        <v>171</v>
+      </c>
+      <c r="D79" s="35"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="32" t="s">
         <v>58</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="D80" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D80" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="30"/>
+      <c r="A81" s="32"/>
       <c r="B81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D81" s="33"/>
+        <v>173</v>
+      </c>
+      <c r="D81" s="34"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="30"/>
+      <c r="A82" s="32"/>
       <c r="B82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D82" s="33"/>
+        <v>174</v>
+      </c>
+      <c r="D82" s="34"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="30"/>
+      <c r="A83" s="32"/>
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D83" s="33"/>
+        <v>176</v>
+      </c>
+      <c r="D83" s="34"/>
     </row>
     <row r="84" spans="1:4" ht="15.75" thickBot="1">
       <c r="A84" s="31"/>
@@ -2710,229 +2710,229 @@
         <v>10</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D84" s="34"/>
+        <v>177</v>
+      </c>
+      <c r="D84" s="35"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="D85" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="D85" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="30"/>
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D86" s="33"/>
+        <v>180</v>
+      </c>
+      <c r="D86" s="34"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="30"/>
+      <c r="A87" s="32"/>
       <c r="B87" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D87" s="33"/>
+        <v>181</v>
+      </c>
+      <c r="D87" s="34"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="30"/>
+      <c r="A88" s="32"/>
       <c r="B88" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="D88" s="33"/>
+        <v>182</v>
+      </c>
+      <c r="D88" s="34"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="35" t="s">
+      <c r="A89" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D89" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="D89" s="42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="35"/>
+      <c r="A90" s="41"/>
       <c r="B90" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D90" s="39"/>
+        <v>184</v>
+      </c>
+      <c r="D90" s="42"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="35"/>
+      <c r="A91" s="41"/>
       <c r="B91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D91" s="39"/>
+        <v>185</v>
+      </c>
+      <c r="D91" s="42"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="35"/>
+      <c r="A92" s="41"/>
       <c r="B92" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D92" s="39"/>
+        <v>186</v>
+      </c>
+      <c r="D92" s="42"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="35" t="s">
+      <c r="A93" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D93" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="D93" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="35"/>
+      <c r="A94" s="41"/>
       <c r="B94" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D94" s="39"/>
+        <v>188</v>
+      </c>
+      <c r="D94" s="42"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="35"/>
+      <c r="A95" s="41"/>
       <c r="B95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D95" s="39"/>
+        <v>189</v>
+      </c>
+      <c r="D95" s="42"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="35"/>
+      <c r="A96" s="41"/>
       <c r="B96" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D96" s="39"/>
+        <v>190</v>
+      </c>
+      <c r="D96" s="42"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="35" t="s">
+      <c r="A97" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D97" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="D97" s="42" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="35"/>
+      <c r="A98" s="41"/>
       <c r="B98" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D98" s="39"/>
+        <v>192</v>
+      </c>
+      <c r="D98" s="42"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="35"/>
+      <c r="A99" s="41"/>
       <c r="B99" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D99" s="39"/>
+        <v>193</v>
+      </c>
+      <c r="D99" s="42"/>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A100" s="36"/>
+      <c r="A100" s="43"/>
       <c r="B100" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D100" s="40"/>
+        <v>194</v>
+      </c>
+      <c r="D100" s="44"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="30" t="s">
+      <c r="A101" s="32" t="s">
         <v>67</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D101" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D101" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="30"/>
+      <c r="A102" s="32"/>
       <c r="B102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D102" s="33"/>
+        <v>198</v>
+      </c>
+      <c r="D102" s="34"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="30"/>
+      <c r="A103" s="32"/>
       <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D103" s="33"/>
+        <v>197</v>
+      </c>
+      <c r="D103" s="34"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="41"/>
+      <c r="A104" s="30"/>
       <c r="B104" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D104" s="42"/>
+        <v>199</v>
+      </c>
+      <c r="D104" s="36"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="29" t="s">
@@ -2942,41 +2942,41 @@
         <v>6</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D105" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D105" s="33" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="30"/>
+      <c r="A106" s="32"/>
       <c r="B106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D106" s="33"/>
+        <v>201</v>
+      </c>
+      <c r="D106" s="34"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="30"/>
+      <c r="A107" s="32"/>
       <c r="B107" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D107" s="33"/>
+        <v>202</v>
+      </c>
+      <c r="D107" s="34"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="41"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D108" s="42"/>
+        <v>203</v>
+      </c>
+      <c r="D108" s="36"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="29" t="s">
@@ -2986,41 +2986,41 @@
         <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D109" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109" s="33" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="30"/>
+      <c r="A110" s="32"/>
       <c r="B110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D110" s="33"/>
+        <v>205</v>
+      </c>
+      <c r="D110" s="34"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="30"/>
+      <c r="A111" s="32"/>
       <c r="B111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D111" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="D111" s="34"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="41"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D112" s="42"/>
+        <v>207</v>
+      </c>
+      <c r="D112" s="36"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="29" t="s">
@@ -3030,41 +3030,41 @@
         <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D113" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="30"/>
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D114" s="33"/>
+        <v>209</v>
+      </c>
+      <c r="D114" s="34"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="30"/>
+      <c r="A115" s="32"/>
       <c r="B115" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D115" s="33"/>
+        <v>210</v>
+      </c>
+      <c r="D115" s="34"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="41"/>
+      <c r="A116" s="30"/>
       <c r="B116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D116" s="42"/>
+        <v>211</v>
+      </c>
+      <c r="D116" s="36"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="29" t="s">
@@ -3074,41 +3074,41 @@
         <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D117" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="D117" s="33" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="30"/>
+      <c r="A118" s="32"/>
       <c r="B118" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D118" s="33"/>
+        <v>196</v>
+      </c>
+      <c r="D118" s="34"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="30"/>
+      <c r="A119" s="32"/>
       <c r="B119" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D119" s="33"/>
+        <v>213</v>
+      </c>
+      <c r="D119" s="34"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="41"/>
+      <c r="A120" s="30"/>
       <c r="B120" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D120" s="42"/>
+        <v>214</v>
+      </c>
+      <c r="D120" s="36"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="29" t="s">
@@ -3118,41 +3118,41 @@
         <v>6</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D121" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D121" s="33" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="30"/>
+      <c r="A122" s="32"/>
       <c r="B122" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D122" s="33"/>
+        <v>216</v>
+      </c>
+      <c r="D122" s="34"/>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="30"/>
+      <c r="A123" s="32"/>
       <c r="B123" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D123" s="33"/>
+        <v>217</v>
+      </c>
+      <c r="D123" s="34"/>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="41"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D124" s="42"/>
+        <v>218</v>
+      </c>
+      <c r="D124" s="36"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="29" t="s">
@@ -3162,41 +3162,41 @@
         <v>6</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D125" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D125" s="33" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="30"/>
+      <c r="A126" s="32"/>
       <c r="B126" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D126" s="33"/>
+        <v>220</v>
+      </c>
+      <c r="D126" s="34"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="30"/>
+      <c r="A127" s="32"/>
       <c r="B127" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D127" s="33"/>
+        <v>221</v>
+      </c>
+      <c r="D127" s="34"/>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="41"/>
+      <c r="A128" s="30"/>
       <c r="B128" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D128" s="42"/>
+        <v>222</v>
+      </c>
+      <c r="D128" s="36"/>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="29" t="s">
@@ -3206,31 +3206,31 @@
         <v>6</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D129" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="D129" s="33" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="30"/>
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D130" s="33"/>
+        <v>224</v>
+      </c>
+      <c r="D130" s="34"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="30"/>
+      <c r="A131" s="32"/>
       <c r="B131" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D131" s="33"/>
+        <v>225</v>
+      </c>
+      <c r="D131" s="34"/>
     </row>
     <row r="132" spans="1:4" ht="15.75" thickBot="1">
       <c r="A132" s="31"/>
@@ -3238,43 +3238,43 @@
         <v>10</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="D132" s="34"/>
+        <v>226</v>
+      </c>
+      <c r="D132" s="35"/>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="30" t="s">
+      <c r="A133" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B133" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D133" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="D133" s="34" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="30"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D134" s="33"/>
+        <v>258</v>
+      </c>
+      <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="41"/>
+      <c r="A135" s="30"/>
       <c r="B135" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D135" s="42"/>
+        <v>259</v>
+      </c>
+      <c r="D135" s="36"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="29" t="s">
@@ -3284,31 +3284,31 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D136" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="D136" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="30"/>
+      <c r="A137" s="32"/>
       <c r="B137" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D137" s="33"/>
+        <v>261</v>
+      </c>
+      <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="41"/>
+      <c r="A138" s="30"/>
       <c r="B138" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D138" s="42"/>
+        <v>262</v>
+      </c>
+      <c r="D138" s="36"/>
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1">
       <c r="A139" s="20" t="s">
@@ -3316,147 +3316,147 @@
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="14" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D139" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="43" t="s">
+      <c r="A140" s="38" t="s">
         <v>93</v>
       </c>
       <c r="B140" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="D140" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="D140" s="34" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="30"/>
+      <c r="A141" s="32"/>
       <c r="B141" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D141" s="33"/>
+        <v>265</v>
+      </c>
+      <c r="D141" s="34"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="41"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D142" s="42"/>
+        <v>266</v>
+      </c>
+      <c r="D142" s="36"/>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="44" t="s">
+      <c r="A143" s="37" t="s">
         <v>94</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D143" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="D143" s="34" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="30"/>
+      <c r="A144" s="32"/>
       <c r="B144" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D144" s="33"/>
+        <v>268</v>
+      </c>
+      <c r="D144" s="34"/>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="41"/>
+      <c r="A145" s="30"/>
       <c r="B145" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D145" s="42"/>
+        <v>269</v>
+      </c>
+      <c r="D145" s="36"/>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="44" t="s">
+      <c r="A146" s="37" t="s">
         <v>96</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D146" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="D146" s="34" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="30"/>
+      <c r="A147" s="32"/>
       <c r="B147" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D147" s="33"/>
+        <v>271</v>
+      </c>
+      <c r="D147" s="34"/>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="41"/>
+      <c r="A148" s="30"/>
       <c r="B148" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D148" s="42"/>
+        <v>272</v>
+      </c>
+      <c r="D148" s="36"/>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="44" t="s">
+      <c r="A149" s="37" t="s">
         <v>95</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D149" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D149" s="34" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c r="A150" s="30"/>
+      <c r="A150" s="32"/>
       <c r="B150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D150" s="33"/>
+        <v>274</v>
+      </c>
+      <c r="D150" s="34"/>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="41"/>
+      <c r="A151" s="30"/>
       <c r="B151" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D151" s="42"/>
+        <v>275</v>
+      </c>
+      <c r="D151" s="36"/>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="29" t="s">
@@ -3466,31 +3466,31 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D152" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D152" s="34" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="30"/>
+      <c r="A153" s="32"/>
       <c r="B153" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D153" s="33"/>
+        <v>277</v>
+      </c>
+      <c r="D153" s="34"/>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="41"/>
+      <c r="A154" s="30"/>
       <c r="B154" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D154" s="42"/>
+        <v>278</v>
+      </c>
+      <c r="D154" s="36"/>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="29" t="s">
@@ -3500,31 +3500,31 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D155" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="D155" s="34" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="30"/>
+      <c r="A156" s="32"/>
       <c r="B156" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D156" s="33"/>
+        <v>280</v>
+      </c>
+      <c r="D156" s="34"/>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="41"/>
+      <c r="A157" s="30"/>
       <c r="B157" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D157" s="42"/>
+        <v>281</v>
+      </c>
+      <c r="D157" s="36"/>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="29" t="s">
@@ -3534,31 +3534,31 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D158" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="D158" s="34" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c r="A159" s="30"/>
+      <c r="A159" s="32"/>
       <c r="B159" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D159" s="33"/>
+        <v>283</v>
+      </c>
+      <c r="D159" s="34"/>
     </row>
     <row r="160" spans="1:4">
-      <c r="A160" s="41"/>
+      <c r="A160" s="30"/>
       <c r="B160" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D160" s="42"/>
+        <v>284</v>
+      </c>
+      <c r="D160" s="36"/>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="29" t="s">
@@ -3568,31 +3568,31 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D161" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="D161" s="34" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="30"/>
+      <c r="A162" s="32"/>
       <c r="B162" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D162" s="33"/>
+        <v>286</v>
+      </c>
+      <c r="D162" s="34"/>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="41"/>
+      <c r="A163" s="30"/>
       <c r="B163" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D163" s="42"/>
+        <v>287</v>
+      </c>
+      <c r="D163" s="36"/>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="29" t="s">
@@ -3602,31 +3602,31 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D164" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="D164" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="30"/>
+      <c r="A165" s="32"/>
       <c r="B165" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D165" s="33"/>
+        <v>289</v>
+      </c>
+      <c r="D165" s="34"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="41"/>
+      <c r="A166" s="30"/>
       <c r="B166" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D166" s="42"/>
+        <v>290</v>
+      </c>
+      <c r="D166" s="36"/>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="29" t="s">
@@ -3636,235 +3636,235 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D167" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="D167" s="34" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="30"/>
+      <c r="A168" s="32"/>
       <c r="B168" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D168" s="33"/>
+        <v>292</v>
+      </c>
+      <c r="D168" s="34"/>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="41"/>
+      <c r="A169" s="30"/>
       <c r="B169" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D169" s="42"/>
+        <v>293</v>
+      </c>
+      <c r="D169" s="36"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="44" t="s">
+      <c r="A170" s="37" t="s">
         <v>103</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D170" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="D170" s="34" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="30"/>
+      <c r="A171" s="32"/>
       <c r="B171" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D171" s="33"/>
+        <v>295</v>
+      </c>
+      <c r="D171" s="34"/>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="41"/>
+      <c r="A172" s="30"/>
       <c r="B172" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D172" s="42"/>
+        <v>296</v>
+      </c>
+      <c r="D172" s="36"/>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="44" t="s">
+      <c r="A173" s="37" t="s">
         <v>104</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D173" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="D173" s="34" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="30"/>
+      <c r="A174" s="32"/>
       <c r="B174" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D174" s="33"/>
+        <v>298</v>
+      </c>
+      <c r="D174" s="34"/>
     </row>
     <row r="175" spans="1:4">
-      <c r="A175" s="41"/>
+      <c r="A175" s="30"/>
       <c r="B175" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D175" s="42"/>
+        <v>299</v>
+      </c>
+      <c r="D175" s="36"/>
     </row>
     <row r="176" spans="1:4">
-      <c r="A176" s="44" t="s">
+      <c r="A176" s="37" t="s">
         <v>106</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D176" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="D176" s="34" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="177" spans="1:4">
-      <c r="A177" s="30"/>
+      <c r="A177" s="32"/>
       <c r="B177" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D177" s="33"/>
+        <v>301</v>
+      </c>
+      <c r="D177" s="34"/>
     </row>
     <row r="178" spans="1:4">
-      <c r="A178" s="41"/>
+      <c r="A178" s="30"/>
       <c r="B178" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D178" s="42"/>
+        <v>302</v>
+      </c>
+      <c r="D178" s="36"/>
     </row>
     <row r="179" spans="1:4">
-      <c r="A179" s="44" t="s">
+      <c r="A179" s="37" t="s">
         <v>105</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D179" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="D179" s="34" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="180" spans="1:4">
-      <c r="A180" s="30"/>
+      <c r="A180" s="32"/>
       <c r="B180" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D180" s="33"/>
+        <v>304</v>
+      </c>
+      <c r="D180" s="34"/>
     </row>
     <row r="181" spans="1:4">
-      <c r="A181" s="41"/>
+      <c r="A181" s="30"/>
       <c r="B181" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D181" s="42"/>
+        <v>305</v>
+      </c>
+      <c r="D181" s="36"/>
     </row>
     <row r="182" spans="1:4">
-      <c r="A182" s="44" t="s">
+      <c r="A182" s="37" t="s">
         <v>107</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D182" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="D182" s="34" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="183" spans="1:4">
-      <c r="A183" s="30"/>
+      <c r="A183" s="32"/>
       <c r="B183" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D183" s="33"/>
+        <v>307</v>
+      </c>
+      <c r="D183" s="34"/>
     </row>
     <row r="184" spans="1:4">
-      <c r="A184" s="41"/>
+      <c r="A184" s="30"/>
       <c r="B184" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D184" s="42"/>
+        <v>308</v>
+      </c>
+      <c r="D184" s="36"/>
     </row>
     <row r="185" spans="1:4">
-      <c r="A185" s="44" t="s">
+      <c r="A185" s="37" t="s">
         <v>108</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D185" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="D185" s="34" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:4">
-      <c r="A186" s="30"/>
+      <c r="A186" s="32"/>
       <c r="B186" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D186" s="33"/>
+        <v>310</v>
+      </c>
+      <c r="D186" s="34"/>
     </row>
     <row r="187" spans="1:4">
-      <c r="A187" s="41"/>
+      <c r="A187" s="30"/>
       <c r="B187" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D187" s="42"/>
+        <v>311</v>
+      </c>
+      <c r="D187" s="36"/>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="29" t="s">
@@ -3874,31 +3874,31 @@
         <v>16</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D188" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="D188" s="34" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="189" spans="1:4">
-      <c r="A189" s="30"/>
+      <c r="A189" s="32"/>
       <c r="B189" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D189" s="33"/>
+        <v>313</v>
+      </c>
+      <c r="D189" s="34"/>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="41"/>
+      <c r="A190" s="30"/>
       <c r="B190" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D190" s="42"/>
+        <v>314</v>
+      </c>
+      <c r="D190" s="36"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="29" t="s">
@@ -3908,21 +3908,21 @@
         <v>16</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D191" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="D191" s="33" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="192" spans="1:4">
-      <c r="A192" s="30"/>
+      <c r="A192" s="32"/>
       <c r="B192" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D192" s="33"/>
+        <v>316</v>
+      </c>
+      <c r="D192" s="34"/>
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1">
       <c r="A193" s="31"/>
@@ -3930,29 +3930,29 @@
         <v>18</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="D193" s="34"/>
+        <v>317</v>
+      </c>
+      <c r="D193" s="35"/>
     </row>
     <row r="194" spans="1:4">
-      <c r="A194" s="30" t="s">
+      <c r="A194" s="32" t="s">
         <v>129</v>
       </c>
       <c r="B194" s="13"/>
       <c r="C194" s="13" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D194" s="27" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="195" spans="1:4">
-      <c r="A195" s="41"/>
+      <c r="A195" s="30"/>
       <c r="B195" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D195" s="19" t="s">
         <v>138</v>
@@ -3963,19 +3963,19 @@
         <v>130</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D196" s="19" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="197" spans="1:4">
-      <c r="A197" s="41"/>
+      <c r="A197" s="30"/>
       <c r="B197" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D197" s="19" t="s">
         <v>140</v>
@@ -3986,19 +3986,19 @@
         <v>131</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D198" s="19" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="199" spans="1:4">
-      <c r="A199" s="41"/>
+      <c r="A199" s="30"/>
       <c r="B199" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D199" s="19" t="s">
         <v>142</v>
@@ -4009,19 +4009,19 @@
         <v>132</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D200" s="19" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="201" spans="1:4">
-      <c r="A201" s="41"/>
+      <c r="A201" s="30"/>
       <c r="B201" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D201" s="19" t="s">
         <v>144</v>
@@ -4032,22 +4032,22 @@
         <v>133</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D202" s="19" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="41"/>
+      <c r="A203" s="30"/>
       <c r="B203" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D203" s="19" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4055,22 +4055,22 @@
         <v>135</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="205" spans="1:4">
-      <c r="A205" s="41"/>
+      <c r="A205" s="30"/>
       <c r="B205" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4078,22 +4078,22 @@
         <v>134</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="D206" s="19" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="41"/>
+      <c r="A207" s="30"/>
       <c r="B207" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D207" s="19" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4101,10 +4101,10 @@
         <v>136</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D208" s="19" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" thickBot="1">
@@ -4113,10 +4113,10 @@
         <v>18</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D209" s="28" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B210" s="13"/>
       <c r="C210" s="13" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D210" s="17" t="s">
         <v>150</v>
@@ -4136,7 +4136,7 @@
         <v>146</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>151</v>
@@ -4147,7 +4147,7 @@
         <v>147</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>152</v>
@@ -4158,7 +4158,7 @@
         <v>148</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>153</v>
@@ -4170,7 +4170,7 @@
       </c>
       <c r="B214" s="11"/>
       <c r="C214" s="11" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D214" s="18" t="s">
         <v>154</v>
@@ -4178,14 +4178,14 @@
     </row>
     <row r="215" spans="1:4" ht="15.75" thickBot="1">
       <c r="A215" s="20" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B215" s="14"/>
       <c r="C215" s="14" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="D215" s="26" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4194,7 +4194,7 @@
       </c>
       <c r="B216" s="13"/>
       <c r="C216" s="13" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D216" s="17" t="s">
         <v>156</v>
@@ -4202,56 +4202,48 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="A204:A205"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="A208:A209"/>
-    <mergeCell ref="A191:A193"/>
-    <mergeCell ref="D191:D193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="D155:D157"/>
-    <mergeCell ref="D152:D154"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="D146:D148"/>
-    <mergeCell ref="D188:D190"/>
-    <mergeCell ref="D185:D187"/>
-    <mergeCell ref="D182:D184"/>
-    <mergeCell ref="D179:D181"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="D173:D175"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A184"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="A158:A160"/>
-    <mergeCell ref="A167:A169"/>
-    <mergeCell ref="A170:A172"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="A149:A151"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="D140:D142"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="D161:D163"/>
-    <mergeCell ref="D158:D160"/>
-    <mergeCell ref="D170:D172"/>
-    <mergeCell ref="A136:A138"/>
-    <mergeCell ref="D136:D138"/>
-    <mergeCell ref="A140:A142"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="D125:D128"/>
-    <mergeCell ref="A129:A132"/>
-    <mergeCell ref="D129:D132"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="D41:D45"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D13:D15"/>
     <mergeCell ref="A85:A88"/>
     <mergeCell ref="D85:D88"/>
     <mergeCell ref="A89:A92"/>
@@ -4274,48 +4266,56 @@
     <mergeCell ref="D105:D108"/>
     <mergeCell ref="A109:A112"/>
     <mergeCell ref="D109:D112"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="D136:D138"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="D125:D128"/>
+    <mergeCell ref="A129:A132"/>
+    <mergeCell ref="D129:D132"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A148"/>
+    <mergeCell ref="A149:A151"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="D140:D142"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="D161:D163"/>
+    <mergeCell ref="D158:D160"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="D155:D157"/>
+    <mergeCell ref="D152:D154"/>
+    <mergeCell ref="D149:D151"/>
+    <mergeCell ref="D146:D148"/>
+    <mergeCell ref="D188:D190"/>
+    <mergeCell ref="D185:D187"/>
+    <mergeCell ref="D182:D184"/>
+    <mergeCell ref="D179:D181"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="D173:D175"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="A158:A160"/>
+    <mergeCell ref="A167:A169"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="D170:D172"/>
+    <mergeCell ref="A200:A201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="A208:A209"/>
+    <mergeCell ref="A191:A193"/>
+    <mergeCell ref="D191:D193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="A196:A197"/>
+    <mergeCell ref="A198:A199"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
NOT, AND, TEST, OR, XOR
Реализованы соответствующие инструкции.
</commit_message>
<xml_diff>
--- a/Codes.xlsx
+++ b/Codes.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="370">
   <si>
     <t>Команда</t>
   </si>
@@ -502,117 +503,6 @@
     <t>00</t>
   </si>
   <si>
-    <t>08 0s</t>
-  </si>
-  <si>
-    <t>08 1s</t>
-  </si>
-  <si>
-    <t>06 8s</t>
-  </si>
-  <si>
-    <t>06 9s</t>
-  </si>
-  <si>
-    <t>06 As</t>
-  </si>
-  <si>
-    <t>06 Bs</t>
-  </si>
-  <si>
-    <t>06 Cs</t>
-  </si>
-  <si>
-    <t>09 0s</t>
-  </si>
-  <si>
-    <t>09 1s</t>
-  </si>
-  <si>
-    <t>09 2s</t>
-  </si>
-  <si>
-    <t>09 3s</t>
-  </si>
-  <si>
-    <t>09 4s</t>
-  </si>
-  <si>
-    <t>09 8s</t>
-  </si>
-  <si>
-    <t>09 9s</t>
-  </si>
-  <si>
-    <t>09 As</t>
-  </si>
-  <si>
-    <t>09 Bs</t>
-  </si>
-  <si>
-    <t>09 Cs</t>
-  </si>
-  <si>
-    <t>09 7s</t>
-  </si>
-  <si>
-    <t>09 Ds</t>
-  </si>
-  <si>
-    <t>09 Es</t>
-  </si>
-  <si>
-    <t>09 5s</t>
-  </si>
-  <si>
-    <t>0A 0s</t>
-  </si>
-  <si>
-    <t>0A 1s</t>
-  </si>
-  <si>
-    <t>0A 2s</t>
-  </si>
-  <si>
-    <t>0A 3s</t>
-  </si>
-  <si>
-    <t>0A 4s</t>
-  </si>
-  <si>
-    <t>0A 5s</t>
-  </si>
-  <si>
-    <t>0A 6s</t>
-  </si>
-  <si>
-    <t>0A 7s</t>
-  </si>
-  <si>
-    <t>0A 8s</t>
-  </si>
-  <si>
-    <t>0A 9s</t>
-  </si>
-  <si>
-    <t>0A As</t>
-  </si>
-  <si>
-    <t>0A Bs</t>
-  </si>
-  <si>
-    <t>0A Cs</t>
-  </si>
-  <si>
-    <t>0A Ds</t>
-  </si>
-  <si>
-    <t>0A Es</t>
-  </si>
-  <si>
-    <t>0A Fs</t>
-  </si>
-  <si>
     <t>0B 0s</t>
   </si>
   <si>
@@ -1178,6 +1068,75 @@
   </si>
   <si>
     <t>09 Bi</t>
+  </si>
+  <si>
+    <t>0A 2i</t>
+  </si>
+  <si>
+    <t>0A 3i</t>
+  </si>
+  <si>
+    <t>0B Сs</t>
+  </si>
+  <si>
+    <t>0C Сs</t>
+  </si>
+  <si>
+    <t>Второй операнд — только байт</t>
+  </si>
+  <si>
+    <t>0D 6z</t>
+  </si>
+  <si>
+    <t>0D 7z</t>
+  </si>
+  <si>
+    <t>0D Az</t>
+  </si>
+  <si>
+    <t>0D Bz</t>
+  </si>
+  <si>
+    <t>0D 4z</t>
+  </si>
+  <si>
+    <t>0D 5z</t>
+  </si>
+  <si>
+    <t>0D 8z</t>
+  </si>
+  <si>
+    <t>0D 9z</t>
+  </si>
+  <si>
+    <t>BTR</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>0E 6z</t>
+  </si>
+  <si>
+    <t>0E 7z</t>
+  </si>
+  <si>
+    <t>0E Az</t>
+  </si>
+  <si>
+    <t>0E Bz</t>
+  </si>
+  <si>
+    <t>0E 4z</t>
+  </si>
+  <si>
+    <t>0E 5z</t>
+  </si>
+  <si>
+    <t>0E 8z</t>
+  </si>
+  <si>
+    <t>0E 9z</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1333,11 +1292,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1406,13 +1374,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1424,14 +1389,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1440,15 +1402,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1456,6 +1418,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1753,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1795,58 +1766,58 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>326</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="D3" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>345</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="32"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D4" s="34"/>
+        <v>301</v>
+      </c>
+      <c r="D4" s="33"/>
       <c r="F4" s="2" t="s">
-        <v>346</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="32"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D5" s="34"/>
+        <v>302</v>
+      </c>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="32"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D6" s="34"/>
+        <v>303</v>
+      </c>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="31"/>
@@ -1854,43 +1825,43 @@
         <v>7</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="D7" s="35"/>
+        <v>304</v>
+      </c>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="D8" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="41"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D9" s="42"/>
+        <v>306</v>
+      </c>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="D10" s="44"/>
+        <v>307</v>
+      </c>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
@@ -1898,7 +1869,7 @@
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>22</v>
@@ -1909,45 +1880,45 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D13" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="41"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D14" s="42"/>
+        <v>290</v>
+      </c>
+      <c r="D14" s="39"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="41"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D15" s="42"/>
+        <v>291</v>
+      </c>
+      <c r="D15" s="39"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10" t="s">
@@ -1955,7 +1926,7 @@
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>21</v>
@@ -1966,7 +1937,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>27</v>
@@ -1980,9 +1951,9 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D18" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1992,499 +1963,499 @@
         <v>17</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="D19" s="35"/>
+        <v>293</v>
+      </c>
+      <c r="D19" s="34"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="D20" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="42" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="41"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D21" s="42"/>
+        <v>295</v>
+      </c>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="35" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D22" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="41"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D23" s="42"/>
+        <v>297</v>
+      </c>
+      <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="35" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D24" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="39" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A25" s="43"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="D25" s="44"/>
+        <v>299</v>
+      </c>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="D26" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="32"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D27" s="34"/>
+        <v>311</v>
+      </c>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="32"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D28" s="34"/>
+        <v>312</v>
+      </c>
+      <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="32"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D29" s="34"/>
+        <v>313</v>
+      </c>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="32"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="D30" s="34"/>
+        <v>314</v>
+      </c>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="35" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D31" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="D31" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="41"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="D32" s="42"/>
+        <v>316</v>
+      </c>
+      <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="41"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D33" s="42"/>
+        <v>317</v>
+      </c>
+      <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="41"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D34" s="42"/>
+        <v>318</v>
+      </c>
+      <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A35" s="43"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="D35" s="44"/>
+        <v>319</v>
+      </c>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>357</v>
-      </c>
-      <c r="D36" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="D36" s="42" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="41"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D37" s="42"/>
+        <v>321</v>
+      </c>
+      <c r="D37" s="39"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="41"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D38" s="42"/>
+        <v>322</v>
+      </c>
+      <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="41"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D39" s="42"/>
+        <v>323</v>
+      </c>
+      <c r="D39" s="39"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="41"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="D40" s="42"/>
+        <v>324</v>
+      </c>
+      <c r="D40" s="39"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D41" s="42" t="s">
+        <v>325</v>
+      </c>
+      <c r="D41" s="39" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="41"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D42" s="42"/>
+        <v>326</v>
+      </c>
+      <c r="D42" s="39"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="41"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D43" s="42"/>
+        <v>327</v>
+      </c>
+      <c r="D43" s="39"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="41"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D44" s="42"/>
+        <v>328</v>
+      </c>
+      <c r="D44" s="39"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A45" s="43"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="D45" s="44"/>
+        <v>329</v>
+      </c>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="43" t="s">
         <v>85</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="D46" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="D46" s="44" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="41"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D47" s="42"/>
+        <v>331</v>
+      </c>
+      <c r="D47" s="39"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="41"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D48" s="42"/>
+        <v>332</v>
+      </c>
+      <c r="D48" s="39"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="41"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D49" s="42"/>
+        <v>333</v>
+      </c>
+      <c r="D49" s="39"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A50" s="43"/>
+      <c r="A50" s="36"/>
       <c r="B50" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D50" s="44"/>
+        <v>334</v>
+      </c>
+      <c r="D50" s="40"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="30" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="30"/>
+      <c r="B52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="32"/>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D52" s="33"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="41"/>
+      <c r="B53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D52" s="34"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="30"/>
-      <c r="B53" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D53" s="36"/>
+        <v>337</v>
+      </c>
+      <c r="D53" s="42"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="30"/>
+      <c r="B55" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D54" s="33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="32"/>
-      <c r="B55" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D55" s="34"/>
+        <v>339</v>
+      </c>
+      <c r="D55" s="33"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1">
       <c r="A56" s="31"/>
       <c r="B56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="D56" s="34"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="D56" s="35"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" s="13" t="s">
+      <c r="C57" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="30"/>
+      <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D57" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="32"/>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D58" s="33"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="41"/>
+      <c r="B59" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D58" s="34"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="30"/>
-      <c r="B59" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D59" s="36"/>
+        <v>343</v>
+      </c>
+      <c r="D59" s="42"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="30"/>
+      <c r="B61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D60" s="33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="32"/>
-      <c r="B61" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D61" s="34"/>
+        <v>345</v>
+      </c>
+      <c r="D61" s="33"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1">
       <c r="A62" s="31"/>
       <c r="B62" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="D62" s="35"/>
+        <v>346</v>
+      </c>
+      <c r="D62" s="34"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D63" s="40" t="s">
+      <c r="C63" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D63" s="38" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2494,447 +2465,465 @@
         <v>17</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="35"/>
+        <v>348</v>
+      </c>
+      <c r="D64" s="34"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="32" t="s">
-        <v>83</v>
+      <c r="A65" s="41" t="s">
+        <v>54</v>
       </c>
       <c r="B65" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="35"/>
+      <c r="B66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D66" s="39"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="35"/>
+      <c r="B67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="32"/>
-      <c r="B66" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D66" s="34"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="32"/>
-      <c r="B67" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" s="34"/>
+        <v>169</v>
+      </c>
+      <c r="D67" s="39"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="32"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="39"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="35"/>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" s="39"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D68" s="34"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="32"/>
-      <c r="B69" s="11" t="s">
+      <c r="D70" s="39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="35"/>
+      <c r="B71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C71" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D69" s="34"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="D71" s="39"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="35"/>
+      <c r="B72" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D70" s="42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="41"/>
-      <c r="B71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D71" s="42"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="41"/>
-      <c r="B72" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D72" s="42"/>
+      <c r="D72" s="39"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="41"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D73" s="42"/>
+      <c r="D73" s="39"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A74" s="43"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D74" s="40"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="30"/>
+      <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D74" s="44"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75" s="13" t="s">
+      <c r="C76" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D76" s="33"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="30"/>
+      <c r="B77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D75" s="34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="32"/>
-      <c r="B76" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D76" s="34"/>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="32"/>
-      <c r="B77" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D77" s="34"/>
+        <v>184</v>
+      </c>
+      <c r="D77" s="33"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="32"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D78" s="34"/>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" s="33"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="41"/>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D79" s="42"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="30"/>
+      <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="D79" s="35"/>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80" s="13" t="s">
+      <c r="C81" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D81" s="33"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="30"/>
+      <c r="B82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D80" s="34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="32"/>
-      <c r="B81" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D81" s="34"/>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="32"/>
-      <c r="B82" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C82" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D82" s="34"/>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="32"/>
+        <v>182</v>
+      </c>
+      <c r="D82" s="33"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="30"/>
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" s="34"/>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1">
+        <v>183</v>
+      </c>
+      <c r="D83" s="33"/>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1">
       <c r="A84" s="31"/>
       <c r="B84" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D84" s="34"/>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D85" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="30"/>
+      <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D84" s="35"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B85" s="13" t="s">
+      <c r="C86" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D86" s="33"/>
+      <c r="E86" s="47"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="30"/>
+      <c r="B87" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="D85" s="40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="32"/>
-      <c r="B86" s="1" t="s">
+      <c r="C87" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D87" s="33"/>
+      <c r="E87" s="47"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="30"/>
+      <c r="B88" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="D88" s="33"/>
+      <c r="E88" s="47"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" s="34"/>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="32"/>
-      <c r="B87" s="1" t="s">
+      <c r="C89" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D89" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E89" s="47"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="35"/>
+      <c r="B90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D90" s="39"/>
+      <c r="E90" s="47"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="35"/>
+      <c r="B91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D91" s="39"/>
+      <c r="E91" s="47"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="35"/>
+      <c r="B92" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D87" s="34"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="32"/>
-      <c r="B88" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D88" s="34"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D89" s="42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="41"/>
-      <c r="B90" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D90" s="42"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="41"/>
-      <c r="B91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D91" s="42"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="41"/>
-      <c r="B92" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C92" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D92" s="42"/>
-    </row>
-    <row r="93" spans="1:4">
+        <v>359</v>
+      </c>
+      <c r="D92" s="39"/>
+      <c r="E92" s="47"/>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E93" s="47"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="35"/>
+      <c r="B94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D94" s="39"/>
+      <c r="E94" s="47"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="35"/>
+      <c r="B95" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D93" s="42" t="s">
+      <c r="C95" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D95" s="39"/>
+      <c r="E95" s="47"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="35"/>
+      <c r="B96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D96" s="39"/>
+      <c r="E96" s="47"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D97" s="32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="41"/>
-      <c r="B94" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D94" s="42"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="41"/>
-      <c r="B95" s="1" t="s">
+      <c r="E97" s="47"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="30"/>
+      <c r="B98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D98" s="33"/>
+      <c r="E98" s="47"/>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="30"/>
+      <c r="B99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D99" s="33"/>
+      <c r="E99" s="47"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A100" s="31"/>
+      <c r="B100" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D95" s="42"/>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="41"/>
-      <c r="B96" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D96" s="42"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="41"/>
-      <c r="B98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D98" s="42"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="41"/>
-      <c r="B99" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D99" s="42"/>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A100" s="43"/>
-      <c r="B100" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="C100" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D100" s="44"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="D100" s="34"/>
+      <c r="E100" s="47"/>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D101" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D101" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="32"/>
+    <row r="102" spans="1:5">
+      <c r="A102" s="30"/>
       <c r="B102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D102" s="34"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="32"/>
+        <v>161</v>
+      </c>
+      <c r="D102" s="33"/>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="30"/>
       <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D103" s="34"/>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="30"/>
+        <v>160</v>
+      </c>
+      <c r="D103" s="33"/>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="41"/>
       <c r="B104" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D104" s="36"/>
-    </row>
-    <row r="105" spans="1:4">
+        <v>162</v>
+      </c>
+      <c r="D104" s="42"/>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="29" t="s">
         <v>69</v>
       </c>
@@ -2942,43 +2931,43 @@
         <v>6</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D105" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D105" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="32"/>
+    <row r="106" spans="1:5">
+      <c r="A106" s="30"/>
       <c r="B106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D106" s="34"/>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="32"/>
+        <v>164</v>
+      </c>
+      <c r="D106" s="33"/>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="30"/>
       <c r="B107" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D107" s="34"/>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="30"/>
+        <v>165</v>
+      </c>
+      <c r="D107" s="33"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="41"/>
       <c r="B108" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D108" s="36"/>
-    </row>
-    <row r="109" spans="1:4">
+        <v>166</v>
+      </c>
+      <c r="D108" s="42"/>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="29" t="s">
         <v>71</v>
       </c>
@@ -2986,41 +2975,41 @@
         <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D109" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D109" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="32"/>
+    <row r="110" spans="1:5">
+      <c r="A110" s="30"/>
       <c r="B110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D110" s="34"/>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="32"/>
+        <v>168</v>
+      </c>
+      <c r="D110" s="33"/>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="30"/>
       <c r="B111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D111" s="34"/>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="30"/>
+        <v>169</v>
+      </c>
+      <c r="D111" s="33"/>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="41"/>
       <c r="B112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D112" s="36"/>
+        <v>170</v>
+      </c>
+      <c r="D112" s="42"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="29" t="s">
@@ -3030,41 +3019,41 @@
         <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D113" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D113" s="32" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="32"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D114" s="34"/>
+        <v>172</v>
+      </c>
+      <c r="D114" s="33"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="32"/>
+      <c r="A115" s="30"/>
       <c r="B115" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D115" s="34"/>
+        <v>173</v>
+      </c>
+      <c r="D115" s="33"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="30"/>
+      <c r="A116" s="41"/>
       <c r="B116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D116" s="36"/>
+        <v>174</v>
+      </c>
+      <c r="D116" s="42"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="29" t="s">
@@ -3074,41 +3063,41 @@
         <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D117" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D117" s="32" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="32"/>
+      <c r="A118" s="30"/>
       <c r="B118" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D118" s="34"/>
+        <v>159</v>
+      </c>
+      <c r="D118" s="33"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="32"/>
+      <c r="A119" s="30"/>
       <c r="B119" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D119" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="D119" s="33"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="30"/>
+      <c r="A120" s="41"/>
       <c r="B120" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D120" s="36"/>
+        <v>177</v>
+      </c>
+      <c r="D120" s="42"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="29" t="s">
@@ -3118,41 +3107,41 @@
         <v>6</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D121" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D121" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="32"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D122" s="34"/>
+        <v>179</v>
+      </c>
+      <c r="D122" s="33"/>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="32"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D123" s="34"/>
+        <v>180</v>
+      </c>
+      <c r="D123" s="33"/>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="30"/>
+      <c r="A124" s="41"/>
       <c r="B124" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D124" s="36"/>
+        <v>181</v>
+      </c>
+      <c r="D124" s="42"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="29" t="s">
@@ -3162,41 +3151,41 @@
         <v>6</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D125" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D125" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="32"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D126" s="34"/>
+        <v>183</v>
+      </c>
+      <c r="D126" s="33"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="32"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D127" s="34"/>
+        <v>184</v>
+      </c>
+      <c r="D127" s="33"/>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="30"/>
+      <c r="A128" s="41"/>
       <c r="B128" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D128" s="36"/>
+        <v>185</v>
+      </c>
+      <c r="D128" s="42"/>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="29" t="s">
@@ -3206,31 +3195,31 @@
         <v>6</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D129" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D129" s="32" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="32"/>
+      <c r="A130" s="30"/>
       <c r="B130" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D130" s="34"/>
+        <v>187</v>
+      </c>
+      <c r="D130" s="33"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="32"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D131" s="34"/>
+        <v>188</v>
+      </c>
+      <c r="D131" s="33"/>
     </row>
     <row r="132" spans="1:4" ht="15.75" thickBot="1">
       <c r="A132" s="31"/>
@@ -3238,43 +3227,43 @@
         <v>10</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D132" s="35"/>
+        <v>189</v>
+      </c>
+      <c r="D132" s="34"/>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="32" t="s">
+      <c r="A133" s="30" t="s">
         <v>87</v>
       </c>
       <c r="B133" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="D133" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="D133" s="33" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="32"/>
+      <c r="A134" s="30"/>
       <c r="B134" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D134" s="34"/>
+        <v>221</v>
+      </c>
+      <c r="D134" s="33"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="30"/>
+      <c r="A135" s="41"/>
       <c r="B135" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D135" s="36"/>
+        <v>222</v>
+      </c>
+      <c r="D135" s="42"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="29" t="s">
@@ -3284,31 +3273,31 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D136" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="D136" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="32"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D137" s="34"/>
+        <v>224</v>
+      </c>
+      <c r="D137" s="33"/>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="30"/>
+      <c r="A138" s="41"/>
       <c r="B138" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D138" s="36"/>
+        <v>225</v>
+      </c>
+      <c r="D138" s="42"/>
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1">
       <c r="A139" s="20" t="s">
@@ -3316,147 +3305,147 @@
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="14" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="D139" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="38" t="s">
+      <c r="A140" s="45" t="s">
         <v>93</v>
       </c>
       <c r="B140" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D140" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="D140" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="32"/>
+      <c r="A141" s="30"/>
       <c r="B141" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D141" s="34"/>
+        <v>228</v>
+      </c>
+      <c r="D141" s="33"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="30"/>
+      <c r="A142" s="41"/>
       <c r="B142" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D142" s="36"/>
+        <v>229</v>
+      </c>
+      <c r="D142" s="42"/>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="37" t="s">
+      <c r="A143" s="46" t="s">
         <v>94</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D143" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="D143" s="33" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="32"/>
+      <c r="A144" s="30"/>
       <c r="B144" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D144" s="34"/>
+        <v>231</v>
+      </c>
+      <c r="D144" s="33"/>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="30"/>
+      <c r="A145" s="41"/>
       <c r="B145" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D145" s="36"/>
+        <v>232</v>
+      </c>
+      <c r="D145" s="42"/>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="37" t="s">
+      <c r="A146" s="46" t="s">
         <v>96</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D146" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D146" s="33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="32"/>
+      <c r="A147" s="30"/>
       <c r="B147" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D147" s="34"/>
+        <v>234</v>
+      </c>
+      <c r="D147" s="33"/>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="30"/>
+      <c r="A148" s="41"/>
       <c r="B148" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D148" s="36"/>
+        <v>235</v>
+      </c>
+      <c r="D148" s="42"/>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="37" t="s">
+      <c r="A149" s="46" t="s">
         <v>95</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D149" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D149" s="33" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c r="A150" s="32"/>
+      <c r="A150" s="30"/>
       <c r="B150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D150" s="34"/>
+        <v>237</v>
+      </c>
+      <c r="D150" s="33"/>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="30"/>
+      <c r="A151" s="41"/>
       <c r="B151" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D151" s="36"/>
+        <v>238</v>
+      </c>
+      <c r="D151" s="42"/>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="29" t="s">
@@ -3466,31 +3455,31 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D152" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D152" s="33" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="32"/>
+      <c r="A153" s="30"/>
       <c r="B153" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D153" s="34"/>
+        <v>240</v>
+      </c>
+      <c r="D153" s="33"/>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="30"/>
+      <c r="A154" s="41"/>
       <c r="B154" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D154" s="36"/>
+        <v>241</v>
+      </c>
+      <c r="D154" s="42"/>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="29" t="s">
@@ -3500,31 +3489,31 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D155" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D155" s="33" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="32"/>
+      <c r="A156" s="30"/>
       <c r="B156" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D156" s="34"/>
+        <v>243</v>
+      </c>
+      <c r="D156" s="33"/>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="30"/>
+      <c r="A157" s="41"/>
       <c r="B157" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D157" s="36"/>
+        <v>244</v>
+      </c>
+      <c r="D157" s="42"/>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="29" t="s">
@@ -3534,31 +3523,31 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D158" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="D158" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c r="A159" s="32"/>
+      <c r="A159" s="30"/>
       <c r="B159" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D159" s="34"/>
+        <v>246</v>
+      </c>
+      <c r="D159" s="33"/>
     </row>
     <row r="160" spans="1:4">
-      <c r="A160" s="30"/>
+      <c r="A160" s="41"/>
       <c r="B160" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D160" s="36"/>
+        <v>247</v>
+      </c>
+      <c r="D160" s="42"/>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="29" t="s">
@@ -3568,31 +3557,31 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D161" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D161" s="33" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="32"/>
+      <c r="A162" s="30"/>
       <c r="B162" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D162" s="34"/>
+        <v>249</v>
+      </c>
+      <c r="D162" s="33"/>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="30"/>
+      <c r="A163" s="41"/>
       <c r="B163" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D163" s="36"/>
+        <v>250</v>
+      </c>
+      <c r="D163" s="42"/>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="29" t="s">
@@ -3602,31 +3591,31 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D164" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="D164" s="33" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="32"/>
+      <c r="A165" s="30"/>
       <c r="B165" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D165" s="34"/>
+        <v>252</v>
+      </c>
+      <c r="D165" s="33"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="30"/>
+      <c r="A166" s="41"/>
       <c r="B166" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D166" s="36"/>
+        <v>253</v>
+      </c>
+      <c r="D166" s="42"/>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="29" t="s">
@@ -3636,235 +3625,235 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D167" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D167" s="33" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="32"/>
+      <c r="A168" s="30"/>
       <c r="B168" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D168" s="34"/>
+        <v>255</v>
+      </c>
+      <c r="D168" s="33"/>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="30"/>
+      <c r="A169" s="41"/>
       <c r="B169" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D169" s="36"/>
+        <v>256</v>
+      </c>
+      <c r="D169" s="42"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="37" t="s">
+      <c r="A170" s="46" t="s">
         <v>103</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D170" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="D170" s="33" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="32"/>
+      <c r="A171" s="30"/>
       <c r="B171" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D171" s="34"/>
+        <v>258</v>
+      </c>
+      <c r="D171" s="33"/>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="30"/>
+      <c r="A172" s="41"/>
       <c r="B172" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D172" s="36"/>
+        <v>259</v>
+      </c>
+      <c r="D172" s="42"/>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="37" t="s">
+      <c r="A173" s="46" t="s">
         <v>104</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D173" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D173" s="33" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="32"/>
+      <c r="A174" s="30"/>
       <c r="B174" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D174" s="34"/>
+        <v>261</v>
+      </c>
+      <c r="D174" s="33"/>
     </row>
     <row r="175" spans="1:4">
-      <c r="A175" s="30"/>
+      <c r="A175" s="41"/>
       <c r="B175" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D175" s="36"/>
+        <v>262</v>
+      </c>
+      <c r="D175" s="42"/>
     </row>
     <row r="176" spans="1:4">
-      <c r="A176" s="37" t="s">
+      <c r="A176" s="46" t="s">
         <v>106</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D176" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="D176" s="33" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="177" spans="1:4">
-      <c r="A177" s="32"/>
+      <c r="A177" s="30"/>
       <c r="B177" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D177" s="34"/>
+        <v>264</v>
+      </c>
+      <c r="D177" s="33"/>
     </row>
     <row r="178" spans="1:4">
-      <c r="A178" s="30"/>
+      <c r="A178" s="41"/>
       <c r="B178" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D178" s="36"/>
+        <v>265</v>
+      </c>
+      <c r="D178" s="42"/>
     </row>
     <row r="179" spans="1:4">
-      <c r="A179" s="37" t="s">
+      <c r="A179" s="46" t="s">
         <v>105</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D179" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="D179" s="33" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="180" spans="1:4">
-      <c r="A180" s="32"/>
+      <c r="A180" s="30"/>
       <c r="B180" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D180" s="34"/>
+        <v>267</v>
+      </c>
+      <c r="D180" s="33"/>
     </row>
     <row r="181" spans="1:4">
-      <c r="A181" s="30"/>
+      <c r="A181" s="41"/>
       <c r="B181" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D181" s="36"/>
+        <v>268</v>
+      </c>
+      <c r="D181" s="42"/>
     </row>
     <row r="182" spans="1:4">
-      <c r="A182" s="37" t="s">
+      <c r="A182" s="46" t="s">
         <v>107</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D182" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D182" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="183" spans="1:4">
-      <c r="A183" s="32"/>
+      <c r="A183" s="30"/>
       <c r="B183" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D183" s="34"/>
+        <v>270</v>
+      </c>
+      <c r="D183" s="33"/>
     </row>
     <row r="184" spans="1:4">
-      <c r="A184" s="30"/>
+      <c r="A184" s="41"/>
       <c r="B184" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D184" s="36"/>
+        <v>271</v>
+      </c>
+      <c r="D184" s="42"/>
     </row>
     <row r="185" spans="1:4">
-      <c r="A185" s="37" t="s">
+      <c r="A185" s="46" t="s">
         <v>108</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D185" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="D185" s="33" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:4">
-      <c r="A186" s="32"/>
+      <c r="A186" s="30"/>
       <c r="B186" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D186" s="34"/>
+        <v>273</v>
+      </c>
+      <c r="D186" s="33"/>
     </row>
     <row r="187" spans="1:4">
-      <c r="A187" s="30"/>
+      <c r="A187" s="41"/>
       <c r="B187" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D187" s="36"/>
+        <v>274</v>
+      </c>
+      <c r="D187" s="42"/>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="29" t="s">
@@ -3874,31 +3863,31 @@
         <v>16</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D188" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D188" s="33" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="189" spans="1:4">
-      <c r="A189" s="32"/>
+      <c r="A189" s="30"/>
       <c r="B189" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D189" s="34"/>
+        <v>276</v>
+      </c>
+      <c r="D189" s="33"/>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="30"/>
+      <c r="A190" s="41"/>
       <c r="B190" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D190" s="36"/>
+        <v>277</v>
+      </c>
+      <c r="D190" s="42"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="29" t="s">
@@ -3908,21 +3897,21 @@
         <v>16</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D191" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="D191" s="32" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="192" spans="1:4">
-      <c r="A192" s="32"/>
+      <c r="A192" s="30"/>
       <c r="B192" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D192" s="34"/>
+        <v>279</v>
+      </c>
+      <c r="D192" s="33"/>
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1">
       <c r="A193" s="31"/>
@@ -3930,29 +3919,29 @@
         <v>18</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D193" s="35"/>
+        <v>280</v>
+      </c>
+      <c r="D193" s="34"/>
     </row>
     <row r="194" spans="1:4">
-      <c r="A194" s="32" t="s">
+      <c r="A194" s="30" t="s">
         <v>129</v>
       </c>
       <c r="B194" s="13"/>
       <c r="C194" s="13" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="D194" s="27" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="195" spans="1:4">
-      <c r="A195" s="30"/>
+      <c r="A195" s="41"/>
       <c r="B195" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="D195" s="19" t="s">
         <v>138</v>
@@ -3963,19 +3952,19 @@
         <v>130</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="D196" s="19" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="197" spans="1:4">
-      <c r="A197" s="30"/>
+      <c r="A197" s="41"/>
       <c r="B197" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="D197" s="19" t="s">
         <v>140</v>
@@ -3986,19 +3975,19 @@
         <v>131</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="D198" s="19" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="199" spans="1:4">
-      <c r="A199" s="30"/>
+      <c r="A199" s="41"/>
       <c r="B199" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="D199" s="19" t="s">
         <v>142</v>
@@ -4009,19 +3998,19 @@
         <v>132</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="D200" s="19" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="201" spans="1:4">
-      <c r="A201" s="30"/>
+      <c r="A201" s="41"/>
       <c r="B201" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="D201" s="19" t="s">
         <v>144</v>
@@ -4032,22 +4021,22 @@
         <v>133</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="D202" s="19" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="30"/>
+      <c r="A203" s="41"/>
       <c r="B203" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="D203" s="19" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4055,22 +4044,22 @@
         <v>135</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
     </row>
     <row r="205" spans="1:4">
-      <c r="A205" s="30"/>
+      <c r="A205" s="41"/>
       <c r="B205" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4078,22 +4067,22 @@
         <v>134</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="D206" s="19" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="30"/>
+      <c r="A207" s="41"/>
       <c r="B207" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="D207" s="19" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4101,10 +4090,10 @@
         <v>136</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="D208" s="19" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" thickBot="1">
@@ -4113,10 +4102,10 @@
         <v>18</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>250</v>
+        <v>213</v>
       </c>
       <c r="D209" s="28" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4125,7 +4114,7 @@
       </c>
       <c r="B210" s="13"/>
       <c r="C210" s="13" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="D210" s="17" t="s">
         <v>150</v>
@@ -4136,7 +4125,7 @@
         <v>146</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>151</v>
@@ -4147,7 +4136,7 @@
         <v>147</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>152</v>
@@ -4158,7 +4147,7 @@
         <v>148</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>153</v>
@@ -4170,7 +4159,7 @@
       </c>
       <c r="B214" s="11"/>
       <c r="C214" s="11" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
       <c r="D214" s="18" t="s">
         <v>154</v>
@@ -4178,14 +4167,14 @@
     </row>
     <row r="215" spans="1:4" ht="15.75" thickBot="1">
       <c r="A215" s="20" t="s">
-        <v>318</v>
+        <v>281</v>
       </c>
       <c r="B215" s="14"/>
       <c r="C215" s="14" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="D215" s="26" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4194,94 +4183,25 @@
       </c>
       <c r="B216" s="13"/>
       <c r="C216" s="13" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
       <c r="D216" s="17" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="D65:D69"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="D85:D88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="D89:D92"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="D93:D96"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="D97:D100"/>
-    <mergeCell ref="A133:A135"/>
-    <mergeCell ref="D133:D135"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="D113:D116"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="D117:D120"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="D121:D124"/>
-    <mergeCell ref="A101:A104"/>
-    <mergeCell ref="D101:D104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="D109:D112"/>
-    <mergeCell ref="A136:A138"/>
-    <mergeCell ref="D136:D138"/>
-    <mergeCell ref="A140:A142"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="D125:D128"/>
-    <mergeCell ref="A129:A132"/>
-    <mergeCell ref="D129:D132"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="A149:A151"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="D140:D142"/>
+  <mergeCells count="115">
+    <mergeCell ref="E85:E100"/>
+    <mergeCell ref="A200:A201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="A208:A209"/>
+    <mergeCell ref="A191:A193"/>
+    <mergeCell ref="D191:D193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="A196:A197"/>
+    <mergeCell ref="A198:A199"/>
     <mergeCell ref="D167:D169"/>
     <mergeCell ref="D164:D166"/>
     <mergeCell ref="D161:D163"/>
@@ -4306,18 +4226,102 @@
     <mergeCell ref="A167:A169"/>
     <mergeCell ref="A170:A172"/>
     <mergeCell ref="D170:D172"/>
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="A204:A205"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="A208:A209"/>
-    <mergeCell ref="A191:A193"/>
-    <mergeCell ref="D191:D193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="A198:A199"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="D136:D138"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="D125:D128"/>
+    <mergeCell ref="A129:A132"/>
+    <mergeCell ref="D129:D132"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A148"/>
+    <mergeCell ref="A149:A151"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="D140:D142"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="D85:D88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="D89:D92"/>
+    <mergeCell ref="A93:A96"/>
+    <mergeCell ref="D93:D96"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="D97:D100"/>
+    <mergeCell ref="A133:A135"/>
+    <mergeCell ref="D133:D135"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="D113:D116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="D117:D120"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="D121:D124"/>
+    <mergeCell ref="A101:A104"/>
+    <mergeCell ref="D101:D104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="D109:D112"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="D41:D45"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="D70:D74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>